<commit_message>
plotMultilayer will be deleted after this (for Release)
- TO-DO comments resolved

- Plotting functions (for Forest and AGriculture) ready for release

- Multilayer plotting merged together out of simulator flow. Will be removed for release after this Push. Then, will be added in near-future versions.

GNU GPL licence and copyright statement aadded to everywhere

- Code standardization and comments finalzied.

- GUI input regulations done

- Transmitter incidence input converted to elevation

- Icons modified with the latest versions

-
</commit_message>
<xml_diff>
--- a/source/input/configuration/default-ss-ml-Tx_var.xlsx
+++ b/source/input/configuration/default-ss-ml-Tx_var.xlsx
@@ -43,9 +43,6 @@
     <t>zB (m)</t>
   </si>
   <si>
-    <t>Tx_th (deg)</t>
-  </si>
-  <si>
     <t>Tx_ph (deg)</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>VSM_40 (cm3/cm3)</t>
+  </si>
+  <si>
+    <t>Tx_el (deg)</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,25 +401,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>